<commit_message>
DDBB acentos + tipo usuario + usuario vendedor
</commit_message>
<xml_diff>
--- a/DDBB/ancalayola_ddbb_TABLAS.xlsx
+++ b/DDBB/ancalayola_ddbb_TABLAS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1 Categorias" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="4 Productos" sheetId="1" r:id="rId4"/>
     <sheet name="Datos" sheetId="3" r:id="rId5"/>
     <sheet name="5 prod INSERT" sheetId="2" r:id="rId6"/>
+    <sheet name="6,1 Tipo Usuarios" sheetId="9" r:id="rId7"/>
+    <sheet name="6,2 Usuarios" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="ingredientes">Datos!$B$3:$B$11</definedName>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="260">
   <si>
     <t>prod_codigo</t>
   </si>
@@ -203,15 +205,9 @@
     <t>p-a</t>
   </si>
   <si>
-    <t>P-Azúcar</t>
-  </si>
-  <si>
     <t>p-k</t>
   </si>
   <si>
-    <t>P-Camarón</t>
-  </si>
-  <si>
     <t>p-cbf</t>
   </si>
   <si>
@@ -311,27 +307,12 @@
     <t>P-3 Quesos</t>
   </si>
   <si>
-    <t>P-Queso-Camarón</t>
-  </si>
-  <si>
     <t>P-Queso-Frijol</t>
   </si>
   <si>
-    <t>P-Queso-Camarón-Frijol</t>
-  </si>
-  <si>
-    <t>P-Bola-Camarón</t>
-  </si>
-  <si>
     <t>P-Bola-Frijol</t>
   </si>
   <si>
-    <t>P-Bola-Camarón-Frijol</t>
-  </si>
-  <si>
-    <t>P-Camarón-Frijol</t>
-  </si>
-  <si>
     <t>Fanta Naranja 600ml</t>
   </si>
   <si>
@@ -581,9 +562,6 @@
     <t>Mezcla de azúcar y queso para relleno de panuchos</t>
   </si>
   <si>
-    <t>Azúcar</t>
-  </si>
-  <si>
     <t>frijol.png</t>
   </si>
   <si>
@@ -599,9 +577,6 @@
     <t>Camaron para relleno de panuchos</t>
   </si>
   <si>
-    <t>Camarón</t>
-  </si>
-  <si>
     <t>bola.png</t>
   </si>
   <si>
@@ -750,13 +725,97 @@
   </si>
   <si>
     <t>Trenza Nutella</t>
+  </si>
+  <si>
+    <t>Camaron</t>
+  </si>
+  <si>
+    <t>Azucar</t>
+  </si>
+  <si>
+    <t>P-Camaron</t>
+  </si>
+  <si>
+    <t>P-Queso-Camaron</t>
+  </si>
+  <si>
+    <t>P-Queso-Camaron-Frijol</t>
+  </si>
+  <si>
+    <t>P-Bola-Camaron</t>
+  </si>
+  <si>
+    <t>P-Bola-Camaron-Frijol</t>
+  </si>
+  <si>
+    <t>P-Camaron-Frijol</t>
+  </si>
+  <si>
+    <t>P-Azucar</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>administrador</t>
+  </si>
+  <si>
+    <t>usuario general con todos los privilegios.</t>
+  </si>
+  <si>
+    <t>tipousuario_codigo</t>
+  </si>
+  <si>
+    <t>tipousuario_nombre</t>
+  </si>
+  <si>
+    <t>tipousuario_notas</t>
+  </si>
+  <si>
+    <t>tipousuario_status</t>
+  </si>
+  <si>
+    <t>vendedor</t>
+  </si>
+  <si>
+    <t>usuarios_nombre</t>
+  </si>
+  <si>
+    <t>usuarios_descripcion</t>
+  </si>
+  <si>
+    <t>usuarios_status</t>
+  </si>
+  <si>
+    <t>usuarios_tipousuario_id</t>
+  </si>
+  <si>
+    <t>JWSK</t>
+  </si>
+  <si>
+    <t>Adminstrador</t>
+  </si>
+  <si>
+    <t>Yola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT INTO usuarios (usuarios_nombre, usuarios_descripcion, usuarios_status, usuarios_tipousuario_id) VALUES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT INTO `tipo_usuario` (`tipousuario_id`, `tipousuario_codigo`, `tipousuario_nombre`, `tipousuario_notas`, `tipousuario_status`) VALUES </t>
+  </si>
+  <si>
+    <t>tipousuario_id</t>
+  </si>
+  <si>
+    <t>Usuario registrado para poder realizar ventas,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -924,8 +983,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1135,8 +1202,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1288,6 +1361,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1333,7 +1419,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1521,6 +1607,18 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1566,7 +1664,40 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1810,26 +1941,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla14" displayName="Tabla14" ref="A1:F9" totalsRowShown="0" headerRowDxfId="33" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla14" displayName="Tabla14" ref="A1:F9" totalsRowShown="0" headerRowDxfId="39" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="6">
     <tableColumn id="1" name="cat_nombre" dataCellStyle="Normal"/>
     <tableColumn id="2" name="cat_codigo" dataCellStyle="Normal"/>
     <tableColumn id="3" name="cat_descripcion" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="cat_padre" dataDxfId="32" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="cat_nivel" dataDxfId="31" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="cat_status" dataDxfId="30" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="cat_padre" dataDxfId="38" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="cat_nivel" dataDxfId="37" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="cat_status" dataDxfId="36" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla25" displayName="Tabla25" ref="A2:D10" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla25" displayName="Tabla25" ref="A2:D10" totalsRowShown="0" headerRowDxfId="35">
   <tableColumns count="4">
     <tableColumn id="1" name="presentacion_codigo"/>
     <tableColumn id="2" name="presentacion_nombre"/>
     <tableColumn id="3" name="presentacion_descripcion"/>
-    <tableColumn id="4" name="presentacion_status" dataDxfId="28"/>
+    <tableColumn id="4" name="presentacion_status" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1842,69 +1973,96 @@
     <tableColumn id="2" name="ingred_codigo"/>
     <tableColumn id="3" name="ingred_ingrediente"/>
     <tableColumn id="4" name="ingred_descripcion"/>
-    <tableColumn id="5" name="ingred_presentacion" dataDxfId="27"/>
+    <tableColumn id="5" name="ingred_presentacion" dataDxfId="33"/>
     <tableColumn id="6" name="ingred_imagen"/>
-    <tableColumn id="7" name="ingred_status" dataDxfId="26"/>
+    <tableColumn id="7" name="ingred_status" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B1:L50" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" dataCellStyle="Notas">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B1:L50" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" dataCellStyle="Notas">
   <tableColumns count="11">
-    <tableColumn id="1" name="prod_codigo" dataDxfId="23"/>
-    <tableColumn id="2" name="prod_nombre" dataDxfId="22"/>
-    <tableColumn id="3" name="prod_categoria" dataDxfId="21"/>
-    <tableColumn id="4" name="prod_creacion" dataDxfId="20"/>
-    <tableColumn id="5" name="prod_precio" dataDxfId="19"/>
-    <tableColumn id="6" name="prod_presentacion" dataDxfId="18"/>
-    <tableColumn id="7" name="prod_ingrediente1" dataDxfId="17" dataCellStyle="Notas"/>
-    <tableColumn id="8" name="prod_ingrediente2" dataDxfId="16" dataCellStyle="Notas"/>
-    <tableColumn id="9" name="prod_ingrediente3" dataDxfId="15" dataCellStyle="Notas"/>
-    <tableColumn id="10" name="prod_status" dataDxfId="14"/>
-    <tableColumn id="11" name="prod_imagen" dataDxfId="13" dataCellStyle="Notas"/>
+    <tableColumn id="1" name="prod_codigo" dataDxfId="29"/>
+    <tableColumn id="2" name="prod_nombre" dataDxfId="28"/>
+    <tableColumn id="3" name="prod_categoria" dataDxfId="27"/>
+    <tableColumn id="4" name="prod_creacion" dataDxfId="26"/>
+    <tableColumn id="5" name="prod_precio" dataDxfId="25"/>
+    <tableColumn id="6" name="prod_presentacion" dataDxfId="24"/>
+    <tableColumn id="7" name="prod_ingrediente1" dataDxfId="23" dataCellStyle="Notas"/>
+    <tableColumn id="8" name="prod_ingrediente2" dataDxfId="22" dataCellStyle="Notas"/>
+    <tableColumn id="9" name="prod_ingrediente3" dataDxfId="21" dataCellStyle="Notas"/>
+    <tableColumn id="10" name="prod_status" dataDxfId="20"/>
+    <tableColumn id="11" name="prod_imagen" dataDxfId="19" dataCellStyle="Notas"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="B1:L50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="B1:L50" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <tableColumns count="11">
-    <tableColumn id="1" name="prod_codigo" dataDxfId="10">
+    <tableColumn id="1" name="prod_codigo" dataDxfId="16">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_codigo]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="prod_nombre" dataDxfId="9">
+    <tableColumn id="2" name="prod_nombre" dataDxfId="15">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="prod_categoria" dataDxfId="8" dataCellStyle="Neutral">
+    <tableColumn id="3" name="prod_categoria" dataDxfId="14" dataCellStyle="Neutral">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_categoria]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="prod_creacion" dataDxfId="7"/>
-    <tableColumn id="5" name="prod_precio" dataDxfId="6">
+    <tableColumn id="4" name="prod_creacion" dataDxfId="13"/>
+    <tableColumn id="5" name="prod_precio" dataDxfId="12">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_precio]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="prod_presentacion" dataDxfId="5" dataCellStyle="Incorrecto">
+    <tableColumn id="6" name="prod_presentacion" dataDxfId="11" dataCellStyle="Incorrecto">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_presentacion]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="prod_ingrediente1" dataDxfId="4">
+    <tableColumn id="7" name="prod_ingrediente1" dataDxfId="10">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_ingrediente1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="prod_ingrediente2" dataDxfId="3" dataCellStyle="Bueno">
+    <tableColumn id="8" name="prod_ingrediente2" dataDxfId="9" dataCellStyle="Bueno">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_ingrediente2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="prod_ingrediente3" dataDxfId="2">
+    <tableColumn id="9" name="prod_ingrediente3" dataDxfId="8">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_ingrediente3]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="prod_status" dataDxfId="1">
+    <tableColumn id="10" name="prod_status" dataDxfId="7">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_status]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="prod_imagen" dataDxfId="0">
+    <tableColumn id="11" name="prod_imagen" dataDxfId="6">
       <calculatedColumnFormula>IF(Tabla1[[#This Row],[prod_imagen]] = 0,"",Tabla1[[#This Row],[prod_imagen]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A2:E4" totalsRowShown="0" headerRowDxfId="0">
+  <tableColumns count="5">
+    <tableColumn id="1" name="tipousuario_id"/>
+    <tableColumn id="2" name="tipousuario_codigo"/>
+    <tableColumn id="3" name="tipousuario_nombre"/>
+    <tableColumn id="4" name="tipousuario_notas" dataDxfId="2"/>
+    <tableColumn id="5" name="tipousuario_status" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="A2:D4" totalsRowShown="0" headerRowDxfId="5">
+  <tableColumns count="4">
+    <tableColumn id="1" name="usuarios_nombre"/>
+    <tableColumn id="2" name="usuarios_descripcion"/>
+    <tableColumn id="3" name="usuarios_status" dataDxfId="4"/>
+    <tableColumn id="4" name="usuarios_tipousuario_id" dataDxfId="3">
+      <calculatedColumnFormula>Tabla6[[#This Row],[tipousuario_id]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2190,39 +2348,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="H1" s="49" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E2" s="48">
         <v>0</v>
@@ -2237,16 +2395,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E3" s="48">
         <v>0</v>
@@ -2261,16 +2419,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E4" s="48">
         <v>0</v>
@@ -2285,13 +2443,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D5" s="48">
         <v>1</v>
@@ -2309,13 +2467,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D6" s="48">
         <v>1</v>
@@ -2333,13 +2491,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D7" s="48">
         <v>1</v>
@@ -2357,13 +2515,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D8" s="48">
         <v>3</v>
@@ -2381,13 +2539,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
         <v>119</v>
-      </c>
-      <c r="B9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" t="s">
-        <v>126</v>
       </c>
       <c r="D9" s="48">
         <v>3</v>
@@ -2431,30 +2589,30 @@
   <sheetData>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -2466,13 +2624,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -2484,13 +2642,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -2502,13 +2660,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -2520,13 +2678,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -2538,13 +2696,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -2556,13 +2714,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -2574,13 +2732,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -2604,7 +2762,7 @@
   <dimension ref="B1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2631,51 +2789,51 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" t="s">
         <v>214</v>
       </c>
-      <c r="D3" t="s">
-        <v>223</v>
-      </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="F3" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="G3" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="H3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="J3" s="38" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="L3" s="38" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E4" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>12</v>
@@ -2691,22 +2849,22 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>12</v>
@@ -2722,22 +2880,22 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>12</v>
@@ -2753,22 +2911,22 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G7" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>12</v>
@@ -2784,22 +2942,22 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G8" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>12</v>
@@ -2815,22 +2973,22 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E9" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G9" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>12</v>
@@ -2846,22 +3004,22 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" t="s">
         <v>181</v>
       </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E10" t="s">
-        <v>189</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G10" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>12</v>
@@ -2872,27 +3030,27 @@
       </c>
       <c r="L10" s="38" t="str">
         <f>CONCATENATE("('",Tabla3[[#This Row],[ingred_tipo]],"', '",Tabla3[[#This Row],[ingred_codigo]],"', '",+Tabla3[[#This Row],[ingred_ingrediente]],"', '",+Tabla3[[#This Row],[ingred_descripcion]],"', ",J10,", '",Tabla3[[#This Row],[ingred_imagen]],"', '",Tabla3[[#This Row],[ingred_status]],"'), ")</f>
-        <v xml:space="preserve">('pedido', 'camaron', 'Camarón', 'Camaron para relleno de panuchos', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'und'), 'camaron.png', 'A'), </v>
+        <v xml:space="preserve">('pedido', 'camaron', 'Camaron', 'Camaron para relleno de panuchos', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'und'), 'camaron.png', 'A'), </v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E11" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G11" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>12</v>
@@ -2908,22 +3066,22 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>233</v>
       </c>
       <c r="E12" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G12" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>12</v>
@@ -2934,30 +3092,30 @@
       </c>
       <c r="L12" s="38" t="str">
         <f>CONCATENATE("('",Tabla3[[#This Row],[ingred_tipo]],"', '",Tabla3[[#This Row],[ingred_codigo]],"', '",+Tabla3[[#This Row],[ingred_ingrediente]],"', '",+Tabla3[[#This Row],[ingred_descripcion]],"', ",J12,", '",Tabla3[[#This Row],[ingred_imagen]],"', '",Tabla3[[#This Row],[ingred_status]],"'), ")</f>
-        <v xml:space="preserve">('pedido', 'azucar', 'Azúcar', 'Mezcla de azúcar y queso para relleno de panuchos', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'und'), 'sugar_cube.png', 'A'), </v>
+        <v xml:space="preserve">('pedido', 'azucar', 'Azucar', 'Mezcla de azúcar y queso para relleno de panuchos', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'und'), 'sugar_cube.png', 'A'), </v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D13" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E13" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G13" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="J13" s="38" t="str">
         <f>CONCATENATE("(SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = '",Tabla3[[#This Row],[ingred_presentacion]],"')")</f>
@@ -2965,7 +3123,7 @@
       </c>
       <c r="L13" s="38" t="str">
         <f>CONCATENATE("('",Tabla3[[#This Row],[ingred_tipo]],"', '",Tabla3[[#This Row],[ingred_codigo]],"', '",+Tabla3[[#This Row],[ingred_ingrediente]],"', '",+Tabla3[[#This Row],[ingred_descripcion]],"', ",J13,", '",Tabla3[[#This Row],[ingred_imagen]],"', '",Tabla3[[#This Row],[ingred_status]],"'), ")</f>
-        <v xml:space="preserve">('pedido', 'manual', 'Manual', 'Pedido de edicion manual', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'indef'), 'manual.png', 'A'), </v>
+        <v xml:space="preserve">('pedido', 'manual', 'Manual', 'Pedido de edicion manual', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'indef'), 'manual.png', 'N'), </v>
       </c>
     </row>
   </sheetData>
@@ -2981,8 +3139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3035,7 +3193,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
@@ -3046,29 +3204,29 @@
         <v>11</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="10">
         <v>45</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="N2"/>
     </row>
@@ -3080,29 +3238,29 @@
         <v>14</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="10">
         <v>23</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N3"/>
     </row>
@@ -3114,29 +3272,29 @@
         <v>16</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="10">
         <v>45</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="N4"/>
     </row>
@@ -3148,29 +3306,29 @@
         <v>18</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="10">
         <v>23</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="N5"/>
     </row>
@@ -3182,29 +3340,29 @@
         <v>20</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="10">
         <v>45</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L6" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="N6"/>
     </row>
@@ -3216,29 +3374,29 @@
         <v>22</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="10">
         <v>23</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L7" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="N7"/>
     </row>
@@ -3250,23 +3408,23 @@
         <v>24</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E8" s="24"/>
       <c r="F8" s="11">
         <v>25</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>12</v>
@@ -3282,23 +3440,23 @@
         <v>32</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="26">
         <v>25</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H9" s="26" t="s">
         <v>26</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K9" s="26" t="s">
         <v>12</v>
@@ -3311,26 +3469,26 @@
         <v>35</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="28">
         <v>30</v>
       </c>
       <c r="G10" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H10" s="29" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K10" s="28" t="s">
         <v>12</v>
@@ -3346,23 +3504,23 @@
         <v>34</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="28">
         <v>30</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H11" s="29" t="s">
         <v>28</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K11" s="28" t="s">
         <v>12</v>
@@ -3375,26 +3533,26 @@
         <v>44</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="28">
         <v>40</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>29</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K12" s="28" t="s">
         <v>12</v>
@@ -3404,29 +3562,29 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>60</v>
+        <v>234</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="28">
         <v>40</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K13" s="28" t="s">
         <v>12</v>
@@ -3442,23 +3600,23 @@
         <v>33</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="28">
         <v>25</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>30</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K14" s="28" t="s">
         <v>12</v>
@@ -3471,26 +3629,26 @@
         <v>57</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>58</v>
+        <v>240</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="28">
         <v>30</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H15" s="29" t="s">
         <v>31</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K15" s="28" t="s">
         <v>12</v>
@@ -3503,17 +3661,17 @@
         <v>40</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="28">
         <v>35</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H16" s="29" t="s">
         <v>25</v>
@@ -3522,7 +3680,7 @@
         <v>26</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K16" s="28" t="s">
         <v>12</v>
@@ -3532,20 +3690,20 @@
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="41" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="42">
         <v>0</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H17" s="44" t="s">
         <v>25</v>
@@ -3554,10 +3712,10 @@
         <v>27</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K17" s="42" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="L17" s="45"/>
       <c r="N17"/>
@@ -3567,17 +3725,17 @@
         <v>39</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="28">
         <v>35</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H18" s="29" t="s">
         <v>25</v>
@@ -3586,7 +3744,7 @@
         <v>28</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K18" s="28" t="s">
         <v>12</v>
@@ -3599,17 +3757,17 @@
         <v>47</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="28">
         <v>45</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H19" s="29" t="s">
         <v>25</v>
@@ -3618,7 +3776,7 @@
         <v>29</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K19" s="28" t="s">
         <v>12</v>
@@ -3631,17 +3789,17 @@
         <v>41</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="28">
         <v>35</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H20" s="29" t="s">
         <v>25</v>
@@ -3650,7 +3808,7 @@
         <v>30</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K20" s="28" t="s">
         <v>12</v>
@@ -3663,17 +3821,17 @@
         <v>46</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="28">
         <v>40</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H21" s="29" t="s">
         <v>25</v>
@@ -3695,17 +3853,17 @@
         <v>36</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="28">
         <v>30</v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H22" s="29" t="s">
         <v>26</v>
@@ -3714,7 +3872,7 @@
         <v>28</v>
       </c>
       <c r="J22" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K22" s="28" t="s">
         <v>12</v>
@@ -3727,17 +3885,17 @@
         <v>51</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="28">
         <v>50</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H23" s="29" t="s">
         <v>26</v>
@@ -3746,7 +3904,7 @@
         <v>29</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K23" s="28" t="s">
         <v>12</v>
@@ -3759,17 +3917,17 @@
         <v>37</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="28">
         <v>30</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>26</v>
@@ -3778,7 +3936,7 @@
         <v>30</v>
       </c>
       <c r="J24" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K24" s="28" t="s">
         <v>12</v>
@@ -3791,17 +3949,17 @@
         <v>45</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="28">
         <v>40</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>26</v>
@@ -3820,20 +3978,20 @@
     </row>
     <row r="26" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E26" s="24"/>
       <c r="F26" s="28">
         <v>45</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H26" s="29" t="s">
         <v>26</v>
@@ -3855,17 +4013,17 @@
         <v>43</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E27" s="24"/>
       <c r="F27" s="28">
         <v>40</v>
       </c>
       <c r="G27" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>27</v>
@@ -3874,7 +4032,7 @@
         <v>28</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K27" s="28" t="s">
         <v>12</v>
@@ -3887,17 +4045,17 @@
         <v>48</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="28">
         <v>45</v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>27</v>
@@ -3906,7 +4064,7 @@
         <v>29</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K28" s="28" t="s">
         <v>12</v>
@@ -3919,17 +4077,17 @@
         <v>42</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="28">
         <v>35</v>
       </c>
       <c r="G29" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H29" s="29" t="s">
         <v>27</v>
@@ -3938,7 +4096,7 @@
         <v>30</v>
       </c>
       <c r="J29" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K29" s="28" t="s">
         <v>12</v>
@@ -3951,17 +4109,17 @@
         <v>50</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="28">
         <v>45</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H30" s="29" t="s">
         <v>27</v>
@@ -3980,20 +4138,20 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="28">
         <v>50</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H31" s="29" t="s">
         <v>27</v>
@@ -4015,17 +4173,17 @@
         <v>49</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="28">
         <v>45</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H32" s="29" t="s">
         <v>28</v>
@@ -4034,7 +4192,7 @@
         <v>29</v>
       </c>
       <c r="J32" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K32" s="28" t="s">
         <v>12</v>
@@ -4044,29 +4202,29 @@
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>94</v>
+        <v>235</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="28">
         <v>50</v>
       </c>
       <c r="G33" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H33" s="29" t="s">
         <v>28</v>
       </c>
       <c r="I33" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J33" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K33" s="28" t="s">
         <v>12</v>
@@ -4076,20 +4234,20 @@
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E34" s="24"/>
       <c r="F34" s="28">
         <v>30</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>28</v>
@@ -4098,7 +4256,7 @@
         <v>30</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K34" s="28" t="s">
         <v>12</v>
@@ -4108,26 +4266,26 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>96</v>
+        <v>236</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E35" s="24"/>
       <c r="F35" s="28">
         <v>55</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H35" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J35" s="11" t="s">
         <v>30</v>
@@ -4140,29 +4298,29 @@
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>97</v>
+        <v>237</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E36" s="24"/>
       <c r="F36" s="28">
         <v>60</v>
       </c>
       <c r="G36" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H36" s="29" t="s">
         <v>29</v>
       </c>
       <c r="I36" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J36" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K36" s="28" t="s">
         <v>12</v>
@@ -4172,20 +4330,20 @@
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E37" s="24"/>
       <c r="F37" s="28">
         <v>45</v>
       </c>
       <c r="G37" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H37" s="29" t="s">
         <v>29</v>
@@ -4194,7 +4352,7 @@
         <v>30</v>
       </c>
       <c r="J37" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K37" s="28" t="s">
         <v>12</v>
@@ -4204,26 +4362,26 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="27" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>99</v>
+        <v>238</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E38" s="24"/>
       <c r="F38" s="28">
         <v>60</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H38" s="29" t="s">
         <v>29</v>
       </c>
       <c r="I38" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J38" s="29" t="s">
         <v>30</v>
@@ -4239,26 +4397,26 @@
         <v>53</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E39" s="24"/>
       <c r="F39" s="28">
         <v>45</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H39" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I39" s="29" t="s">
         <v>30</v>
       </c>
       <c r="J39" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K39" s="28" t="s">
         <v>12</v>
@@ -4268,335 +4426,335 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="30" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C40" s="30" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E40" s="32"/>
       <c r="F40" s="31">
         <v>20</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H40" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I40" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J40" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K40" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N40"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="30" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E41" s="32"/>
       <c r="F41" s="31">
         <v>20</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I41" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K41" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L41" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="N41"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="30" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E42" s="32"/>
       <c r="F42" s="31">
         <v>20</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H42" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K42" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L42" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="N42"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="30" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E43" s="32"/>
       <c r="F43" s="31">
         <v>15</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="H43" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I43" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J43" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K43" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L43" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="N43"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="30" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E44" s="32"/>
       <c r="F44" s="31">
         <v>10</v>
       </c>
       <c r="G44" s="31" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H44" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I44" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J44" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K44" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L44" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="N44"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="30" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E45" s="32"/>
       <c r="F45" s="31">
         <v>50</v>
       </c>
       <c r="G45" s="31" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="H45" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I45" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J45" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K45" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L45" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="N45"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="13">
         <v>20</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H46" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I46" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K46" s="13" t="s">
         <v>12</v>
       </c>
       <c r="L46" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="N46"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E47" s="17"/>
       <c r="F47" s="13">
         <v>20</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H47" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I47" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K47" s="13" t="s">
         <v>12</v>
       </c>
       <c r="L47" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="N47"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="35" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E48" s="37"/>
       <c r="F48" s="36">
         <v>20</v>
       </c>
       <c r="G48" s="36" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H48" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I48" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J48" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K48" s="36" t="s">
         <v>12</v>
       </c>
       <c r="L48" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="N48"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>52</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E49" s="46"/>
       <c r="F49" s="16">
         <v>10</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H49" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I49" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K49" s="16" t="s">
         <v>12</v>
@@ -4605,29 +4763,29 @@
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="13">
         <v>15</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J50" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K50" s="13" t="s">
         <v>12</v>
@@ -4669,7 +4827,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -4680,7 +4838,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -4691,7 +4849,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -4702,7 +4860,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -4713,7 +4871,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -4724,18 +4882,18 @@
         <v>5</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="40">
         <v>6</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -4746,7 +4904,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -4757,12 +4915,12 @@
         <v>9</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="61" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4775,8 +4933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2:X50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4837,30 +4995,30 @@
         <v>9</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N1" s="59" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="O1" s="59"/>
       <c r="P1" s="60" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="Q1" s="59"/>
       <c r="R1" s="59" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="S1" s="59"/>
       <c r="T1" s="59" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="U1" s="59"/>
       <c r="V1" s="59" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="W1" s="59"/>
       <c r="X1" s="40" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
@@ -5651,7 +5809,7 @@
       </c>
       <c r="C13" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Camarón</v>
+        <v>P-Camaron</v>
       </c>
       <c r="D13" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -5712,7 +5870,7 @@
       <c r="W13" s="56"/>
       <c r="X13" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N13,", ",Tabla2[[#This Row],[prod_precio]],", ",P13,", ",R13,", ",T13,", ",V13,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-k', 'P-Camarón', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 40, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-k', 'P-Camaron', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 40, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
@@ -5793,7 +5951,7 @@
       </c>
       <c r="C15" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Azúcar</v>
+        <v>P-Azucar</v>
       </c>
       <c r="D15" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -5854,7 +6012,7 @@
       <c r="W15" s="56"/>
       <c r="X15" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N15,", ",Tabla2[[#This Row],[prod_precio]],", ",P15,", ",R15,", ",T15,", ",V15,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-a', 'P-Azúcar', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 30, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'azucar') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-a', 'P-Azucar', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 30, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'azucar') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
@@ -7071,7 +7229,7 @@
       </c>
       <c r="C33" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Queso-Camarón</v>
+        <v>P-Queso-Camaron</v>
       </c>
       <c r="D33" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7132,7 +7290,7 @@
       <c r="W33" s="56"/>
       <c r="X33" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N33,", ",Tabla2[[#This Row],[prod_precio]],", ",P33,", ",R33,", ",T33,", ",V33,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-qk', 'P-Queso-Camarón', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 50, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'queso') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-qk', 'P-Queso-Camaron', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 50, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'queso') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
@@ -7213,7 +7371,7 @@
       </c>
       <c r="C35" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Queso-Camarón-Frijol</v>
+        <v>P-Queso-Camaron-Frijol</v>
       </c>
       <c r="D35" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7274,7 +7432,7 @@
       <c r="W35" s="56"/>
       <c r="X35" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N35,", ",Tabla2[[#This Row],[prod_precio]],", ",P35,", ",R35,", ",T35,", ",V35,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-qkf', 'P-Queso-Camarón-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 55, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'queso') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , 'A', ''), </v>
+        <v xml:space="preserve">('p-qkf', 'P-Queso-Camaron-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 55, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'queso') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , 'A', ''), </v>
       </c>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.25">
@@ -7284,7 +7442,7 @@
       </c>
       <c r="C36" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Bola-Camarón</v>
+        <v>P-Bola-Camaron</v>
       </c>
       <c r="D36" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7345,7 +7503,7 @@
       <c r="W36" s="56"/>
       <c r="X36" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N36,", ",Tabla2[[#This Row],[prod_precio]],", ",P36,", ",R36,", ",T36,", ",V36,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-bk', 'P-Bola-Camarón', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 60, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'bola') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-bk', 'P-Bola-Camaron', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 60, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'bola') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
@@ -7426,7 +7584,7 @@
       </c>
       <c r="C38" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Bola-Camarón-Frijol</v>
+        <v>P-Bola-Camaron-Frijol</v>
       </c>
       <c r="D38" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7487,7 +7645,7 @@
       <c r="W38" s="56"/>
       <c r="X38" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N38,", ",Tabla2[[#This Row],[prod_precio]],", ",P38,", ",R38,", ",T38,", ",V38,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-bkf', 'P-Bola-Camarón-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 60, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'bola') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , 'A', ''), </v>
+        <v xml:space="preserve">('p-bkf', 'P-Bola-Camaron-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 60, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'bola') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , 'A', ''), </v>
       </c>
     </row>
     <row r="39" spans="2:24" x14ac:dyDescent="0.25">
@@ -7497,7 +7655,7 @@
       </c>
       <c r="C39" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Camarón-Frijol</v>
+        <v>P-Camaron-Frijol</v>
       </c>
       <c r="D39" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7558,7 +7716,7 @@
       <c r="W39" s="56"/>
       <c r="X39" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N39,", ",Tabla2[[#This Row],[prod_precio]],", ",P39,", ",R39,", ",T39,", ",V39,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-kf', 'P-Camarón-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 45, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-kf', 'P-Camaron-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 45, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
@@ -8353,4 +8511,197 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="61"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="69" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="70" t="str">
+        <f>CONCATENATE("(",Tabla6[[#This Row],[tipousuario_id]],", '",Tabla6[[#This Row],[tipousuario_codigo]],"', '",Tabla6[[#This Row],[tipousuario_nombre]],"', '",Tabla6[[#This Row],[tipousuario_notas]],"'),")</f>
+        <v>(1001, 'admin', 'administrador', 'usuario general con todos los privilegios.'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="70" t="str">
+        <f>CONCATENATE("(",Tabla6[[#This Row],[tipousuario_id]],", '",Tabla6[[#This Row],[tipousuario_codigo]],"', '",Tabla6[[#This Row],[tipousuario_nombre]],"', '",Tabla6[[#This Row],[tipousuario_notas]],"'),")</f>
+        <v>(1002, 'vendedor', 'vendedor', 'Usuario registrado para poder realizar ventas,'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="72"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="71" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>256</v>
+      </c>
+      <c r="I2" s="50"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2">
+        <f>Tabla6[[#This Row],[tipousuario_id]]</f>
+        <v>1001</v>
+      </c>
+      <c r="F3" s="51" t="str">
+        <f>CONCATENATE("(SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '",Tabla7[[#This Row],[usuarios_tipousuario_id]],"')")</f>
+        <v>(SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '1001')</v>
+      </c>
+      <c r="H3" t="str">
+        <f>CONCATENATE("('",Tabla7[[#This Row],[usuarios_nombre]],"', '",Tabla7[[#This Row],[usuarios_descripcion]],"', '",Tabla7[[#This Row],[usuarios_status]],"', ",F3,"),")</f>
+        <v>('JWSK', 'Adminstrador', 'A', (SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '1001')),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <f>Tabla6[[#This Row],[tipousuario_id]]</f>
+        <v>1002</v>
+      </c>
+      <c r="F4" s="51" t="str">
+        <f>CONCATENATE("(SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '",Tabla7[[#This Row],[usuarios_tipousuario_id]],"')")</f>
+        <v>(SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '1002')</v>
+      </c>
+      <c r="H4" t="str">
+        <f>CONCATENATE("('",Tabla7[[#This Row],[usuarios_nombre]],"', '",Tabla7[[#This Row],[usuarios_descripcion]],"', '",Tabla7[[#This Row],[usuarios_status]],"', ",F4,"),")</f>
+        <v>('Yola', 'Adminstrador', 'A', (SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '1002')),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ddbb cambios tipo_usuario script
</commit_message>
<xml_diff>
--- a/DDBB/ancalayola_ddbb_TABLAS.xlsx
+++ b/DDBB/ancalayola_ddbb_TABLAS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1 Categorias" sheetId="6" r:id="rId1"/>
@@ -802,13 +802,13 @@
     <t xml:space="preserve">INSERT INTO usuarios (usuarios_nombre, usuarios_descripcion, usuarios_status, usuarios_tipousuario_id) VALUES </t>
   </si>
   <si>
-    <t xml:space="preserve">INSERT INTO `tipo_usuario` (`tipousuario_id`, `tipousuario_codigo`, `tipousuario_nombre`, `tipousuario_notas`, `tipousuario_status`) VALUES </t>
-  </si>
-  <si>
     <t>tipousuario_id</t>
   </si>
   <si>
-    <t>Usuario registrado para poder realizar ventas,</t>
+    <t xml:space="preserve">INSERT INTO tipo_usuario ( tipousuario_id, tipousuario_codigo, tipousuario_nombre, tipousuario_notas, tipousuario_status) VALUES </t>
+  </si>
+  <si>
+    <t>Usuario registrado para poder realizar ventas.</t>
   </si>
 </sst>
 </file>
@@ -1666,6 +1666,21 @@
   </cellStyles>
   <dxfs count="40">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1681,21 +1696,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2040,25 +2040,25 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A2:E4" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A2:E4" totalsRowShown="0" headerRowDxfId="5">
   <tableColumns count="5">
     <tableColumn id="1" name="tipousuario_id"/>
     <tableColumn id="2" name="tipousuario_codigo"/>
     <tableColumn id="3" name="tipousuario_nombre"/>
-    <tableColumn id="4" name="tipousuario_notas" dataDxfId="2"/>
-    <tableColumn id="5" name="tipousuario_status" dataDxfId="1"/>
+    <tableColumn id="4" name="tipousuario_notas" dataDxfId="4"/>
+    <tableColumn id="5" name="tipousuario_status" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="A2:D4" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="A2:D4" totalsRowShown="0" headerRowDxfId="2">
   <tableColumns count="4">
     <tableColumn id="1" name="usuarios_nombre"/>
     <tableColumn id="2" name="usuarios_descripcion"/>
-    <tableColumn id="3" name="usuarios_status" dataDxfId="4"/>
-    <tableColumn id="4" name="usuarios_tipousuario_id" dataDxfId="3">
+    <tableColumn id="3" name="usuarios_status" dataDxfId="1"/>
+    <tableColumn id="4" name="usuarios_tipousuario_id" dataDxfId="0">
       <calculatedColumnFormula>Tabla6[[#This Row],[tipousuario_id]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8517,8 +8517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8536,7 +8536,7 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>244</v>
@@ -8551,7 +8551,7 @@
         <v>247</v>
       </c>
       <c r="G2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -8571,8 +8571,8 @@
         <v>12</v>
       </c>
       <c r="G3" s="70" t="str">
-        <f>CONCATENATE("(",Tabla6[[#This Row],[tipousuario_id]],", '",Tabla6[[#This Row],[tipousuario_codigo]],"', '",Tabla6[[#This Row],[tipousuario_nombre]],"', '",Tabla6[[#This Row],[tipousuario_notas]],"'),")</f>
-        <v>(1001, 'admin', 'administrador', 'usuario general con todos los privilegios.'),</v>
+        <f>CONCATENATE("(",Tabla6[[#This Row],[tipousuario_id]],", '",Tabla6[[#This Row],[tipousuario_codigo]],"', '",Tabla6[[#This Row],[tipousuario_nombre]],"', '",Tabla6[[#This Row],[tipousuario_notas]],"', '",Tabla6[[#This Row],[tipousuario_status]],"'), ")</f>
+        <v xml:space="preserve">(1001, 'admin', 'administrador', 'usuario general con todos los privilegios.', 'A'), </v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8592,8 +8592,8 @@
         <v>12</v>
       </c>
       <c r="G4" s="70" t="str">
-        <f>CONCATENATE("(",Tabla6[[#This Row],[tipousuario_id]],", '",Tabla6[[#This Row],[tipousuario_codigo]],"', '",Tabla6[[#This Row],[tipousuario_nombre]],"', '",Tabla6[[#This Row],[tipousuario_notas]],"'),")</f>
-        <v>(1002, 'vendedor', 'vendedor', 'Usuario registrado para poder realizar ventas,'),</v>
+        <f>CONCATENATE("(",Tabla6[[#This Row],[tipousuario_id]],", '",Tabla6[[#This Row],[tipousuario_codigo]],"', '",Tabla6[[#This Row],[tipousuario_nombre]],"', '",Tabla6[[#This Row],[tipousuario_notas]],"', '",Tabla6[[#This Row],[tipousuario_status]],"'), ")</f>
+        <v xml:space="preserve">(1002, 'vendedor', 'vendedor', 'Usuario registrado para poder realizar ventas.', 'A'), </v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -8612,8 +8612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DDBB actualizada y sinc con 'main'
</commit_message>
<xml_diff>
--- a/DDBB/ancalayola_ddbb_TABLAS.xlsx
+++ b/DDBB/ancalayola_ddbb_TABLAS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1 Categorias" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="4 Productos" sheetId="1" r:id="rId4"/>
     <sheet name="Datos" sheetId="3" r:id="rId5"/>
     <sheet name="5 prod INSERT" sheetId="2" r:id="rId6"/>
+    <sheet name="6,1 Tipo Usuarios" sheetId="9" r:id="rId7"/>
+    <sheet name="6,2 Usuarios" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="ingredientes">Datos!$B$3:$B$11</definedName>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="260">
   <si>
     <t>prod_codigo</t>
   </si>
@@ -203,15 +205,9 @@
     <t>p-a</t>
   </si>
   <si>
-    <t>P-Azúcar</t>
-  </si>
-  <si>
     <t>p-k</t>
   </si>
   <si>
-    <t>P-Camarón</t>
-  </si>
-  <si>
     <t>p-cbf</t>
   </si>
   <si>
@@ -311,27 +307,12 @@
     <t>P-3 Quesos</t>
   </si>
   <si>
-    <t>P-Queso-Camarón</t>
-  </si>
-  <si>
     <t>P-Queso-Frijol</t>
   </si>
   <si>
-    <t>P-Queso-Camarón-Frijol</t>
-  </si>
-  <si>
-    <t>P-Bola-Camarón</t>
-  </si>
-  <si>
     <t>P-Bola-Frijol</t>
   </si>
   <si>
-    <t>P-Bola-Camarón-Frijol</t>
-  </si>
-  <si>
-    <t>P-Camarón-Frijol</t>
-  </si>
-  <si>
     <t>Fanta Naranja 600ml</t>
   </si>
   <si>
@@ -581,9 +562,6 @@
     <t>Mezcla de azúcar y queso para relleno de panuchos</t>
   </si>
   <si>
-    <t>Azúcar</t>
-  </si>
-  <si>
     <t>frijol.png</t>
   </si>
   <si>
@@ -599,9 +577,6 @@
     <t>Camaron para relleno de panuchos</t>
   </si>
   <si>
-    <t>Camarón</t>
-  </si>
-  <si>
     <t>bola.png</t>
   </si>
   <si>
@@ -750,13 +725,97 @@
   </si>
   <si>
     <t>Trenza Nutella</t>
+  </si>
+  <si>
+    <t>Camaron</t>
+  </si>
+  <si>
+    <t>Azucar</t>
+  </si>
+  <si>
+    <t>P-Camaron</t>
+  </si>
+  <si>
+    <t>P-Queso-Camaron</t>
+  </si>
+  <si>
+    <t>P-Queso-Camaron-Frijol</t>
+  </si>
+  <si>
+    <t>P-Bola-Camaron</t>
+  </si>
+  <si>
+    <t>P-Bola-Camaron-Frijol</t>
+  </si>
+  <si>
+    <t>P-Camaron-Frijol</t>
+  </si>
+  <si>
+    <t>P-Azucar</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>administrador</t>
+  </si>
+  <si>
+    <t>usuario general con todos los privilegios.</t>
+  </si>
+  <si>
+    <t>tipousuario_codigo</t>
+  </si>
+  <si>
+    <t>tipousuario_nombre</t>
+  </si>
+  <si>
+    <t>tipousuario_notas</t>
+  </si>
+  <si>
+    <t>tipousuario_status</t>
+  </si>
+  <si>
+    <t>vendedor</t>
+  </si>
+  <si>
+    <t>usuarios_nombre</t>
+  </si>
+  <si>
+    <t>usuarios_descripcion</t>
+  </si>
+  <si>
+    <t>usuarios_status</t>
+  </si>
+  <si>
+    <t>usuarios_tipousuario_id</t>
+  </si>
+  <si>
+    <t>JWSK</t>
+  </si>
+  <si>
+    <t>Adminstrador</t>
+  </si>
+  <si>
+    <t>Yola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT INTO usuarios (usuarios_nombre, usuarios_descripcion, usuarios_status, usuarios_tipousuario_id) VALUES </t>
+  </si>
+  <si>
+    <t>tipousuario_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT INTO tipo_usuario ( tipousuario_id, tipousuario_codigo, tipousuario_nombre, tipousuario_notas, tipousuario_status) VALUES </t>
+  </si>
+  <si>
+    <t>Usuario registrado para poder realizar ventas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -924,8 +983,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1135,8 +1202,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1288,6 +1361,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1333,7 +1419,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1521,6 +1607,18 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1566,7 +1664,40 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="40">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1810,26 +1941,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla14" displayName="Tabla14" ref="A1:F9" totalsRowShown="0" headerRowDxfId="33" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla14" displayName="Tabla14" ref="A1:F9" totalsRowShown="0" headerRowDxfId="39" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="6">
     <tableColumn id="1" name="cat_nombre" dataCellStyle="Normal"/>
     <tableColumn id="2" name="cat_codigo" dataCellStyle="Normal"/>
     <tableColumn id="3" name="cat_descripcion" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="cat_padre" dataDxfId="32" dataCellStyle="Normal"/>
-    <tableColumn id="5" name="cat_nivel" dataDxfId="31" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="cat_status" dataDxfId="30" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="cat_padre" dataDxfId="38" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="cat_nivel" dataDxfId="37" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="cat_status" dataDxfId="36" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla25" displayName="Tabla25" ref="A2:D10" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla25" displayName="Tabla25" ref="A2:D10" totalsRowShown="0" headerRowDxfId="35">
   <tableColumns count="4">
     <tableColumn id="1" name="presentacion_codigo"/>
     <tableColumn id="2" name="presentacion_nombre"/>
     <tableColumn id="3" name="presentacion_descripcion"/>
-    <tableColumn id="4" name="presentacion_status" dataDxfId="28"/>
+    <tableColumn id="4" name="presentacion_status" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1842,69 +1973,96 @@
     <tableColumn id="2" name="ingred_codigo"/>
     <tableColumn id="3" name="ingred_ingrediente"/>
     <tableColumn id="4" name="ingred_descripcion"/>
-    <tableColumn id="5" name="ingred_presentacion" dataDxfId="27"/>
+    <tableColumn id="5" name="ingred_presentacion" dataDxfId="33"/>
     <tableColumn id="6" name="ingred_imagen"/>
-    <tableColumn id="7" name="ingred_status" dataDxfId="26"/>
+    <tableColumn id="7" name="ingred_status" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B1:L50" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" dataCellStyle="Notas">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B1:L50" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" dataCellStyle="Notas">
   <tableColumns count="11">
-    <tableColumn id="1" name="prod_codigo" dataDxfId="23"/>
-    <tableColumn id="2" name="prod_nombre" dataDxfId="22"/>
-    <tableColumn id="3" name="prod_categoria" dataDxfId="21"/>
-    <tableColumn id="4" name="prod_creacion" dataDxfId="20"/>
-    <tableColumn id="5" name="prod_precio" dataDxfId="19"/>
-    <tableColumn id="6" name="prod_presentacion" dataDxfId="18"/>
-    <tableColumn id="7" name="prod_ingrediente1" dataDxfId="17" dataCellStyle="Notas"/>
-    <tableColumn id="8" name="prod_ingrediente2" dataDxfId="16" dataCellStyle="Notas"/>
-    <tableColumn id="9" name="prod_ingrediente3" dataDxfId="15" dataCellStyle="Notas"/>
-    <tableColumn id="10" name="prod_status" dataDxfId="14"/>
-    <tableColumn id="11" name="prod_imagen" dataDxfId="13" dataCellStyle="Notas"/>
+    <tableColumn id="1" name="prod_codigo" dataDxfId="29"/>
+    <tableColumn id="2" name="prod_nombre" dataDxfId="28"/>
+    <tableColumn id="3" name="prod_categoria" dataDxfId="27"/>
+    <tableColumn id="4" name="prod_creacion" dataDxfId="26"/>
+    <tableColumn id="5" name="prod_precio" dataDxfId="25"/>
+    <tableColumn id="6" name="prod_presentacion" dataDxfId="24"/>
+    <tableColumn id="7" name="prod_ingrediente1" dataDxfId="23" dataCellStyle="Notas"/>
+    <tableColumn id="8" name="prod_ingrediente2" dataDxfId="22" dataCellStyle="Notas"/>
+    <tableColumn id="9" name="prod_ingrediente3" dataDxfId="21" dataCellStyle="Notas"/>
+    <tableColumn id="10" name="prod_status" dataDxfId="20"/>
+    <tableColumn id="11" name="prod_imagen" dataDxfId="19" dataCellStyle="Notas"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="B1:L50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="B1:L50" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <tableColumns count="11">
-    <tableColumn id="1" name="prod_codigo" dataDxfId="10">
+    <tableColumn id="1" name="prod_codigo" dataDxfId="16">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_codigo]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="prod_nombre" dataDxfId="9">
+    <tableColumn id="2" name="prod_nombre" dataDxfId="15">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_nombre]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="prod_categoria" dataDxfId="8" dataCellStyle="Neutral">
+    <tableColumn id="3" name="prod_categoria" dataDxfId="14" dataCellStyle="Neutral">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_categoria]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="prod_creacion" dataDxfId="7"/>
-    <tableColumn id="5" name="prod_precio" dataDxfId="6">
+    <tableColumn id="4" name="prod_creacion" dataDxfId="13"/>
+    <tableColumn id="5" name="prod_precio" dataDxfId="12">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_precio]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="prod_presentacion" dataDxfId="5" dataCellStyle="Incorrecto">
+    <tableColumn id="6" name="prod_presentacion" dataDxfId="11" dataCellStyle="Incorrecto">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_presentacion]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="prod_ingrediente1" dataDxfId="4">
+    <tableColumn id="7" name="prod_ingrediente1" dataDxfId="10">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_ingrediente1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="prod_ingrediente2" dataDxfId="3" dataCellStyle="Bueno">
+    <tableColumn id="8" name="prod_ingrediente2" dataDxfId="9" dataCellStyle="Bueno">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_ingrediente2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="prod_ingrediente3" dataDxfId="2">
+    <tableColumn id="9" name="prod_ingrediente3" dataDxfId="8">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_ingrediente3]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="prod_status" dataDxfId="1">
+    <tableColumn id="10" name="prod_status" dataDxfId="7">
       <calculatedColumnFormula>Tabla1[[#This Row],[prod_status]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="prod_imagen" dataDxfId="0">
+    <tableColumn id="11" name="prod_imagen" dataDxfId="6">
       <calculatedColumnFormula>IF(Tabla1[[#This Row],[prod_imagen]] = 0,"",Tabla1[[#This Row],[prod_imagen]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A2:E4" totalsRowShown="0" headerRowDxfId="5">
+  <tableColumns count="5">
+    <tableColumn id="1" name="tipousuario_id"/>
+    <tableColumn id="2" name="tipousuario_codigo"/>
+    <tableColumn id="3" name="tipousuario_nombre"/>
+    <tableColumn id="4" name="tipousuario_notas" dataDxfId="4"/>
+    <tableColumn id="5" name="tipousuario_status" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="A2:D4" totalsRowShown="0" headerRowDxfId="2">
+  <tableColumns count="4">
+    <tableColumn id="1" name="usuarios_nombre"/>
+    <tableColumn id="2" name="usuarios_descripcion"/>
+    <tableColumn id="3" name="usuarios_status" dataDxfId="1"/>
+    <tableColumn id="4" name="usuarios_tipousuario_id" dataDxfId="0">
+      <calculatedColumnFormula>Tabla6[[#This Row],[tipousuario_id]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2190,39 +2348,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="H1" s="49" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E2" s="48">
         <v>0</v>
@@ -2237,16 +2395,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E3" s="48">
         <v>0</v>
@@ -2261,16 +2419,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E4" s="48">
         <v>0</v>
@@ -2285,13 +2443,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D5" s="48">
         <v>1</v>
@@ -2309,13 +2467,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D6" s="48">
         <v>1</v>
@@ -2333,13 +2491,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D7" s="48">
         <v>1</v>
@@ -2357,13 +2515,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D8" s="48">
         <v>3</v>
@@ -2381,13 +2539,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
         <v>119</v>
-      </c>
-      <c r="B9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" t="s">
-        <v>126</v>
       </c>
       <c r="D9" s="48">
         <v>3</v>
@@ -2431,30 +2589,30 @@
   <sheetData>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -2466,13 +2624,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -2484,13 +2642,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -2502,13 +2660,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -2520,13 +2678,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -2538,13 +2696,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -2556,13 +2714,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -2574,13 +2732,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -2604,7 +2762,7 @@
   <dimension ref="B1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2631,51 +2789,51 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" t="s">
         <v>214</v>
       </c>
-      <c r="D3" t="s">
-        <v>223</v>
-      </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="F3" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="G3" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="H3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="J3" s="38" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="L3" s="38" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E4" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>12</v>
@@ -2691,22 +2849,22 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>12</v>
@@ -2722,22 +2880,22 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>12</v>
@@ -2753,22 +2911,22 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G7" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>12</v>
@@ -2784,22 +2942,22 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G8" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>12</v>
@@ -2815,22 +2973,22 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E9" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G9" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>12</v>
@@ -2846,22 +3004,22 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" t="s">
         <v>181</v>
       </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E10" t="s">
-        <v>189</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G10" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>12</v>
@@ -2872,27 +3030,27 @@
       </c>
       <c r="L10" s="38" t="str">
         <f>CONCATENATE("('",Tabla3[[#This Row],[ingred_tipo]],"', '",Tabla3[[#This Row],[ingred_codigo]],"', '",+Tabla3[[#This Row],[ingred_ingrediente]],"', '",+Tabla3[[#This Row],[ingred_descripcion]],"', ",J10,", '",Tabla3[[#This Row],[ingred_imagen]],"', '",Tabla3[[#This Row],[ingred_status]],"'), ")</f>
-        <v xml:space="preserve">('pedido', 'camaron', 'Camarón', 'Camaron para relleno de panuchos', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'und'), 'camaron.png', 'A'), </v>
+        <v xml:space="preserve">('pedido', 'camaron', 'Camaron', 'Camaron para relleno de panuchos', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'und'), 'camaron.png', 'A'), </v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E11" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G11" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>12</v>
@@ -2908,22 +3066,22 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>233</v>
       </c>
       <c r="E12" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G12" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>12</v>
@@ -2934,30 +3092,30 @@
       </c>
       <c r="L12" s="38" t="str">
         <f>CONCATENATE("('",Tabla3[[#This Row],[ingred_tipo]],"', '",Tabla3[[#This Row],[ingred_codigo]],"', '",+Tabla3[[#This Row],[ingred_ingrediente]],"', '",+Tabla3[[#This Row],[ingred_descripcion]],"', ",J12,", '",Tabla3[[#This Row],[ingred_imagen]],"', '",Tabla3[[#This Row],[ingred_status]],"'), ")</f>
-        <v xml:space="preserve">('pedido', 'azucar', 'Azúcar', 'Mezcla de azúcar y queso para relleno de panuchos', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'und'), 'sugar_cube.png', 'A'), </v>
+        <v xml:space="preserve">('pedido', 'azucar', 'Azucar', 'Mezcla de azúcar y queso para relleno de panuchos', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'und'), 'sugar_cube.png', 'A'), </v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D13" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E13" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G13" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="J13" s="38" t="str">
         <f>CONCATENATE("(SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = '",Tabla3[[#This Row],[ingred_presentacion]],"')")</f>
@@ -2965,7 +3123,7 @@
       </c>
       <c r="L13" s="38" t="str">
         <f>CONCATENATE("('",Tabla3[[#This Row],[ingred_tipo]],"', '",Tabla3[[#This Row],[ingred_codigo]],"', '",+Tabla3[[#This Row],[ingred_ingrediente]],"', '",+Tabla3[[#This Row],[ingred_descripcion]],"', ",J13,", '",Tabla3[[#This Row],[ingred_imagen]],"', '",Tabla3[[#This Row],[ingred_status]],"'), ")</f>
-        <v xml:space="preserve">('pedido', 'manual', 'Manual', 'Pedido de edicion manual', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'indef'), 'manual.png', 'A'), </v>
+        <v xml:space="preserve">('pedido', 'manual', 'Manual', 'Pedido de edicion manual', (SELECT presentacion_id FROM presentacion WHERE presentacion_codigo = 'indef'), 'manual.png', 'N'), </v>
       </c>
     </row>
   </sheetData>
@@ -2981,8 +3139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3035,7 +3193,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
@@ -3046,29 +3204,29 @@
         <v>11</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="10">
         <v>45</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="N2"/>
     </row>
@@ -3080,29 +3238,29 @@
         <v>14</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="10">
         <v>23</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="N3"/>
     </row>
@@ -3114,29 +3272,29 @@
         <v>16</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="10">
         <v>45</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="N4"/>
     </row>
@@ -3148,29 +3306,29 @@
         <v>18</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="10">
         <v>23</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="N5"/>
     </row>
@@ -3182,29 +3340,29 @@
         <v>20</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="10">
         <v>45</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L6" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="N6"/>
     </row>
@@ -3216,29 +3374,29 @@
         <v>22</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="10">
         <v>23</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="L7" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="N7"/>
     </row>
@@ -3250,23 +3408,23 @@
         <v>24</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E8" s="24"/>
       <c r="F8" s="11">
         <v>25</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>12</v>
@@ -3282,23 +3440,23 @@
         <v>32</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="26">
         <v>25</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H9" s="26" t="s">
         <v>26</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K9" s="26" t="s">
         <v>12</v>
@@ -3311,26 +3469,26 @@
         <v>35</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="28">
         <v>30</v>
       </c>
       <c r="G10" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H10" s="29" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K10" s="28" t="s">
         <v>12</v>
@@ -3346,23 +3504,23 @@
         <v>34</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="28">
         <v>30</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H11" s="29" t="s">
         <v>28</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K11" s="28" t="s">
         <v>12</v>
@@ -3375,26 +3533,26 @@
         <v>44</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="28">
         <v>40</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>29</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K12" s="28" t="s">
         <v>12</v>
@@ -3404,29 +3562,29 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>60</v>
+        <v>234</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="28">
         <v>40</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K13" s="28" t="s">
         <v>12</v>
@@ -3442,23 +3600,23 @@
         <v>33</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="28">
         <v>25</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>30</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K14" s="28" t="s">
         <v>12</v>
@@ -3471,26 +3629,26 @@
         <v>57</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>58</v>
+        <v>240</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="28">
         <v>30</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H15" s="29" t="s">
         <v>31</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K15" s="28" t="s">
         <v>12</v>
@@ -3503,17 +3661,17 @@
         <v>40</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="28">
         <v>35</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H16" s="29" t="s">
         <v>25</v>
@@ -3522,7 +3680,7 @@
         <v>26</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K16" s="28" t="s">
         <v>12</v>
@@ -3532,20 +3690,20 @@
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="41" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="42">
         <v>0</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H17" s="44" t="s">
         <v>25</v>
@@ -3554,10 +3712,10 @@
         <v>27</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K17" s="42" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="L17" s="45"/>
       <c r="N17"/>
@@ -3567,17 +3725,17 @@
         <v>39</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="28">
         <v>35</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H18" s="29" t="s">
         <v>25</v>
@@ -3586,7 +3744,7 @@
         <v>28</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K18" s="28" t="s">
         <v>12</v>
@@ -3599,17 +3757,17 @@
         <v>47</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="28">
         <v>45</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H19" s="29" t="s">
         <v>25</v>
@@ -3618,7 +3776,7 @@
         <v>29</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K19" s="28" t="s">
         <v>12</v>
@@ -3631,17 +3789,17 @@
         <v>41</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="28">
         <v>35</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H20" s="29" t="s">
         <v>25</v>
@@ -3650,7 +3808,7 @@
         <v>30</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K20" s="28" t="s">
         <v>12</v>
@@ -3663,17 +3821,17 @@
         <v>46</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="28">
         <v>40</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H21" s="29" t="s">
         <v>25</v>
@@ -3695,17 +3853,17 @@
         <v>36</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="28">
         <v>30</v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H22" s="29" t="s">
         <v>26</v>
@@ -3714,7 +3872,7 @@
         <v>28</v>
       </c>
       <c r="J22" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K22" s="28" t="s">
         <v>12</v>
@@ -3727,17 +3885,17 @@
         <v>51</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="28">
         <v>50</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H23" s="29" t="s">
         <v>26</v>
@@ -3746,7 +3904,7 @@
         <v>29</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K23" s="28" t="s">
         <v>12</v>
@@ -3759,17 +3917,17 @@
         <v>37</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="28">
         <v>30</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>26</v>
@@ -3778,7 +3936,7 @@
         <v>30</v>
       </c>
       <c r="J24" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K24" s="28" t="s">
         <v>12</v>
@@ -3791,17 +3949,17 @@
         <v>45</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="28">
         <v>40</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>26</v>
@@ -3820,20 +3978,20 @@
     </row>
     <row r="26" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E26" s="24"/>
       <c r="F26" s="28">
         <v>45</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H26" s="29" t="s">
         <v>26</v>
@@ -3855,17 +4013,17 @@
         <v>43</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E27" s="24"/>
       <c r="F27" s="28">
         <v>40</v>
       </c>
       <c r="G27" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>27</v>
@@ -3874,7 +4032,7 @@
         <v>28</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K27" s="28" t="s">
         <v>12</v>
@@ -3887,17 +4045,17 @@
         <v>48</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="28">
         <v>45</v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>27</v>
@@ -3906,7 +4064,7 @@
         <v>29</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K28" s="28" t="s">
         <v>12</v>
@@ -3919,17 +4077,17 @@
         <v>42</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="28">
         <v>35</v>
       </c>
       <c r="G29" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H29" s="29" t="s">
         <v>27</v>
@@ -3938,7 +4096,7 @@
         <v>30</v>
       </c>
       <c r="J29" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K29" s="28" t="s">
         <v>12</v>
@@ -3951,17 +4109,17 @@
         <v>50</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="28">
         <v>45</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H30" s="29" t="s">
         <v>27</v>
@@ -3980,20 +4138,20 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="28">
         <v>50</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H31" s="29" t="s">
         <v>27</v>
@@ -4015,17 +4173,17 @@
         <v>49</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="28">
         <v>45</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H32" s="29" t="s">
         <v>28</v>
@@ -4034,7 +4192,7 @@
         <v>29</v>
       </c>
       <c r="J32" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K32" s="28" t="s">
         <v>12</v>
@@ -4044,29 +4202,29 @@
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>94</v>
+        <v>235</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="28">
         <v>50</v>
       </c>
       <c r="G33" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H33" s="29" t="s">
         <v>28</v>
       </c>
       <c r="I33" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J33" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K33" s="28" t="s">
         <v>12</v>
@@ -4076,20 +4234,20 @@
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E34" s="24"/>
       <c r="F34" s="28">
         <v>30</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>28</v>
@@ -4098,7 +4256,7 @@
         <v>30</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K34" s="28" t="s">
         <v>12</v>
@@ -4108,26 +4266,26 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>96</v>
+        <v>236</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E35" s="24"/>
       <c r="F35" s="28">
         <v>55</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H35" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J35" s="11" t="s">
         <v>30</v>
@@ -4140,29 +4298,29 @@
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>97</v>
+        <v>237</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E36" s="24"/>
       <c r="F36" s="28">
         <v>60</v>
       </c>
       <c r="G36" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H36" s="29" t="s">
         <v>29</v>
       </c>
       <c r="I36" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J36" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K36" s="28" t="s">
         <v>12</v>
@@ -4172,20 +4330,20 @@
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E37" s="24"/>
       <c r="F37" s="28">
         <v>45</v>
       </c>
       <c r="G37" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H37" s="29" t="s">
         <v>29</v>
@@ -4194,7 +4352,7 @@
         <v>30</v>
       </c>
       <c r="J37" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K37" s="28" t="s">
         <v>12</v>
@@ -4204,26 +4362,26 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="27" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>99</v>
+        <v>238</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E38" s="24"/>
       <c r="F38" s="28">
         <v>60</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H38" s="29" t="s">
         <v>29</v>
       </c>
       <c r="I38" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J38" s="29" t="s">
         <v>30</v>
@@ -4239,26 +4397,26 @@
         <v>53</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E39" s="24"/>
       <c r="F39" s="28">
         <v>45</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H39" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I39" s="29" t="s">
         <v>30</v>
       </c>
       <c r="J39" s="29" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K39" s="28" t="s">
         <v>12</v>
@@ -4268,335 +4426,335 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="30" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C40" s="30" t="s">
         <v>23</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E40" s="32"/>
       <c r="F40" s="31">
         <v>20</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H40" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I40" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J40" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K40" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N40"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="30" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E41" s="32"/>
       <c r="F41" s="31">
         <v>20</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I41" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K41" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L41" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="N41"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="30" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E42" s="32"/>
       <c r="F42" s="31">
         <v>20</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H42" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K42" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L42" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="N42"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="30" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E43" s="32"/>
       <c r="F43" s="31">
         <v>15</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="H43" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I43" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J43" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K43" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L43" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="N43"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="30" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E44" s="32"/>
       <c r="F44" s="31">
         <v>10</v>
       </c>
       <c r="G44" s="31" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H44" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I44" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J44" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K44" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L44" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="N44"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="30" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E45" s="32"/>
       <c r="F45" s="31">
         <v>50</v>
       </c>
       <c r="G45" s="31" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="H45" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I45" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J45" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K45" s="31" t="s">
         <v>12</v>
       </c>
       <c r="L45" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="N45"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="13">
         <v>20</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H46" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I46" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K46" s="13" t="s">
         <v>12</v>
       </c>
       <c r="L46" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="N46"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E47" s="17"/>
       <c r="F47" s="13">
         <v>20</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H47" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I47" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K47" s="13" t="s">
         <v>12</v>
       </c>
       <c r="L47" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="N47"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="35" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E48" s="37"/>
       <c r="F48" s="36">
         <v>20</v>
       </c>
       <c r="G48" s="36" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H48" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I48" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J48" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K48" s="36" t="s">
         <v>12</v>
       </c>
       <c r="L48" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="N48"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>52</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E49" s="46"/>
       <c r="F49" s="16">
         <v>10</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H49" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I49" s="31" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K49" s="16" t="s">
         <v>12</v>
@@ -4605,29 +4763,29 @@
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="13">
         <v>15</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J50" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K50" s="13" t="s">
         <v>12</v>
@@ -4669,7 +4827,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -4680,7 +4838,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -4691,7 +4849,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -4702,7 +4860,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -4713,7 +4871,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -4724,18 +4882,18 @@
         <v>5</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="40">
         <v>6</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -4746,7 +4904,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -4757,12 +4915,12 @@
         <v>9</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="61" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4775,8 +4933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2:X50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4837,30 +4995,30 @@
         <v>9</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N1" s="59" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="O1" s="59"/>
       <c r="P1" s="60" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="Q1" s="59"/>
       <c r="R1" s="59" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="S1" s="59"/>
       <c r="T1" s="59" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="U1" s="59"/>
       <c r="V1" s="59" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="W1" s="59"/>
       <c r="X1" s="40" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
@@ -5651,7 +5809,7 @@
       </c>
       <c r="C13" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Camarón</v>
+        <v>P-Camaron</v>
       </c>
       <c r="D13" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -5712,7 +5870,7 @@
       <c r="W13" s="56"/>
       <c r="X13" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N13,", ",Tabla2[[#This Row],[prod_precio]],", ",P13,", ",R13,", ",T13,", ",V13,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-k', 'P-Camarón', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 40, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-k', 'P-Camaron', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 40, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
@@ -5793,7 +5951,7 @@
       </c>
       <c r="C15" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Azúcar</v>
+        <v>P-Azucar</v>
       </c>
       <c r="D15" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -5854,7 +6012,7 @@
       <c r="W15" s="56"/>
       <c r="X15" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N15,", ",Tabla2[[#This Row],[prod_precio]],", ",P15,", ",R15,", ",T15,", ",V15,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-a', 'P-Azúcar', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 30, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'azucar') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-a', 'P-Azucar', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 30, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'azucar') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
@@ -7071,7 +7229,7 @@
       </c>
       <c r="C33" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Queso-Camarón</v>
+        <v>P-Queso-Camaron</v>
       </c>
       <c r="D33" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7132,7 +7290,7 @@
       <c r="W33" s="56"/>
       <c r="X33" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N33,", ",Tabla2[[#This Row],[prod_precio]],", ",P33,", ",R33,", ",T33,", ",V33,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-qk', 'P-Queso-Camarón', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 50, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'queso') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-qk', 'P-Queso-Camaron', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 50, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'queso') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
@@ -7213,7 +7371,7 @@
       </c>
       <c r="C35" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Queso-Camarón-Frijol</v>
+        <v>P-Queso-Camaron-Frijol</v>
       </c>
       <c r="D35" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7274,7 +7432,7 @@
       <c r="W35" s="56"/>
       <c r="X35" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N35,", ",Tabla2[[#This Row],[prod_precio]],", ",P35,", ",R35,", ",T35,", ",V35,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-qkf', 'P-Queso-Camarón-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 55, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'queso') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , 'A', ''), </v>
+        <v xml:space="preserve">('p-qkf', 'P-Queso-Camaron-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 55, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'queso') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , 'A', ''), </v>
       </c>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.25">
@@ -7284,7 +7442,7 @@
       </c>
       <c r="C36" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Bola-Camarón</v>
+        <v>P-Bola-Camaron</v>
       </c>
       <c r="D36" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7345,7 +7503,7 @@
       <c r="W36" s="56"/>
       <c r="X36" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N36,", ",Tabla2[[#This Row],[prod_precio]],", ",P36,", ",R36,", ",T36,", ",V36,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-bk', 'P-Bola-Camarón', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 60, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'bola') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-bk', 'P-Bola-Camaron', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 60, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'bola') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
@@ -7426,7 +7584,7 @@
       </c>
       <c r="C38" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Bola-Camarón-Frijol</v>
+        <v>P-Bola-Camaron-Frijol</v>
       </c>
       <c r="D38" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7487,7 +7645,7 @@
       <c r="W38" s="56"/>
       <c r="X38" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N38,", ",Tabla2[[#This Row],[prod_precio]],", ",P38,", ",R38,", ",T38,", ",V38,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-bkf', 'P-Bola-Camarón-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 60, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'bola') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , 'A', ''), </v>
+        <v xml:space="preserve">('p-bkf', 'P-Bola-Camaron-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 60, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'bola') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , 'A', ''), </v>
       </c>
     </row>
     <row r="39" spans="2:24" x14ac:dyDescent="0.25">
@@ -7497,7 +7655,7 @@
       </c>
       <c r="C39" t="str">
         <f>Tabla1[[#This Row],[prod_nombre]]</f>
-        <v>P-Camarón-Frijol</v>
+        <v>P-Camaron-Frijol</v>
       </c>
       <c r="D39" s="52" t="str">
         <f>Tabla1[[#This Row],[prod_categoria]]</f>
@@ -7558,7 +7716,7 @@
       <c r="W39" s="56"/>
       <c r="X39" t="str">
         <f>CONCATENATE("('",Tabla2[[#This Row],[prod_codigo]],"', '",Tabla2[[#This Row],[prod_nombre]],"', ",N39,", ",Tabla2[[#This Row],[prod_precio]],", ",P39,", ",R39,", ",T39,", ",V39,", '",Tabla2[[#This Row],[prod_status]],"', '",Tabla2[[#This Row],[prod_imagen]],"'), ")</f>
-        <v xml:space="preserve">('p-kf', 'P-Camarón-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 45, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
+        <v xml:space="preserve">('p-kf', 'P-Camaron-Frijol', (SELECT cat_id FROM categorias WHERE cat_status = 'A' AND cat_codigo = 'P'), 45, (SELECT presentacion_id FROM presentacion WHERE presentacion_status = 'A' AND presentacion_codigo = 'und') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'camaron') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'frijol') , (SELECT ingred_id FROM ingredientes WHERE ingred_status = 'A' AND ingred_codigo = 'indef') , 'A', ''), </v>
       </c>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
@@ -8353,4 +8511,197 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="61"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="69" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="70" t="str">
+        <f>CONCATENATE("(",Tabla6[[#This Row],[tipousuario_id]],", '",Tabla6[[#This Row],[tipousuario_codigo]],"', '",Tabla6[[#This Row],[tipousuario_nombre]],"', '",Tabla6[[#This Row],[tipousuario_notas]],"', '",Tabla6[[#This Row],[tipousuario_status]],"'), ")</f>
+        <v xml:space="preserve">(1001, 'admin', 'administrador', 'usuario general con todos los privilegios.', 'A'), </v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="70" t="str">
+        <f>CONCATENATE("(",Tabla6[[#This Row],[tipousuario_id]],", '",Tabla6[[#This Row],[tipousuario_codigo]],"', '",Tabla6[[#This Row],[tipousuario_nombre]],"', '",Tabla6[[#This Row],[tipousuario_notas]],"', '",Tabla6[[#This Row],[tipousuario_status]],"'), ")</f>
+        <v xml:space="preserve">(1002, 'vendedor', 'vendedor', 'Usuario registrado para poder realizar ventas.', 'A'), </v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="72"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="71" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>256</v>
+      </c>
+      <c r="I2" s="50"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2">
+        <f>Tabla6[[#This Row],[tipousuario_id]]</f>
+        <v>1001</v>
+      </c>
+      <c r="F3" s="51" t="str">
+        <f>CONCATENATE("(SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '",Tabla7[[#This Row],[usuarios_tipousuario_id]],"')")</f>
+        <v>(SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '1001')</v>
+      </c>
+      <c r="H3" t="str">
+        <f>CONCATENATE("('",Tabla7[[#This Row],[usuarios_nombre]],"', '",Tabla7[[#This Row],[usuarios_descripcion]],"', '",Tabla7[[#This Row],[usuarios_status]],"', ",F3,"),")</f>
+        <v>('JWSK', 'Adminstrador', 'A', (SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '1001')),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <f>Tabla6[[#This Row],[tipousuario_id]]</f>
+        <v>1002</v>
+      </c>
+      <c r="F4" s="51" t="str">
+        <f>CONCATENATE("(SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '",Tabla7[[#This Row],[usuarios_tipousuario_id]],"')")</f>
+        <v>(SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '1002')</v>
+      </c>
+      <c r="H4" t="str">
+        <f>CONCATENATE("('",Tabla7[[#This Row],[usuarios_nombre]],"', '",Tabla7[[#This Row],[usuarios_descripcion]],"', '",Tabla7[[#This Row],[usuarios_status]],"', ",F4,"),")</f>
+        <v>('Yola', 'Adminstrador', 'A', (SELECT tipousuario_id FROM tipo_usuario WHERE tipousuario_codigo = '1002')),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>